<commit_message>
re-sorted and grouped results
git-svn-id: https://svnserver.informatik.kit.edu/i43/svn/code@4921 769cc9a0-fb0c-0410-8c2f-a2305f0e6268
</commit_message>
<xml_diff>
--- a/FileShare/results/BytecodePrediction.xlsx
+++ b/FileShare/results/BytecodePrediction.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Vorhersage p0.pdf" sheetId="3" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Vorhersage p0.pdf'!$A$1:$F$38</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -556,7 +559,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -700,6 +703,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -745,7 +815,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -837,9 +907,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="4" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -901,6 +968,30 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="22" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1241,24 +1332,24 @@
   <dimension ref="A1:XEL38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="34" customWidth="1"/>
-    <col min="4" max="4" width="14" style="52" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="34" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="52" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="33" customWidth="1"/>
+    <col min="4" max="4" width="14" style="51" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="33" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="51" customWidth="1"/>
     <col min="7" max="7" width="4.28515625" style="23" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" style="23" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" style="23" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="78" customHeight="1">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="78" customHeight="1" thickBot="1">
       <c r="A1" s="6" t="s">
         <v>34</v>
       </c>
@@ -1282,10 +1373,10 @@
       <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="53">
         <v>44419</v>
       </c>
       <c r="D2" s="13">
@@ -1307,10 +1398,10 @@
       <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="54">
         <v>20114</v>
       </c>
       <c r="D3" s="20">
@@ -1336,10 +1427,10 @@
       <c r="A4" s="17">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="54">
         <v>664051</v>
       </c>
       <c r="D4" s="20">
@@ -1360,14 +1451,14 @@
         <v>81545</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1">
       <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="55">
         <v>20114</v>
       </c>
       <c r="D5" s="20">
@@ -1416,7 +1507,7 @@
       <c r="E7" s="14"/>
       <c r="F7" s="30"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1">
       <c r="A8" s="17">
         <v>7</v>
       </c>
@@ -1435,10 +1526,10 @@
       <c r="A9" s="17">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="53">
         <v>38831</v>
       </c>
       <c r="D9" s="20">
@@ -1457,10 +1548,10 @@
       <c r="A10" s="17">
         <v>9</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="54">
         <v>14247</v>
       </c>
       <c r="D10" s="20">
@@ -1475,14 +1566,14 @@
         <v>26304</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" ht="15.75" thickBot="1">
       <c r="A11" s="17">
         <v>10</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="55">
         <v>19277</v>
       </c>
       <c r="D11" s="20">
@@ -1497,14 +1588,14 @@
         <v>810</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="16" customFormat="1">
+    <row r="12" spans="1:9" s="16" customFormat="1" ht="15.75" thickBot="1">
       <c r="A12" s="10">
         <v>11</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="56"/>
       <c r="D12" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1512,14 +1603,14 @@
       <c r="E12" s="14"/>
       <c r="F12" s="30"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" ht="15.75" thickBot="1">
       <c r="A13" s="17">
         <v>12</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="57">
         <v>6146</v>
       </c>
       <c r="D13" s="20">
@@ -1532,7 +1623,7 @@
       </c>
       <c r="F13" s="29"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1">
       <c r="A14" s="17">
         <v>13</v>
       </c>
@@ -1551,10 +1642,10 @@
       <c r="A15" s="17">
         <v>14</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="53">
         <v>12013</v>
       </c>
       <c r="D15" s="20">
@@ -1571,10 +1662,10 @@
       <c r="A16" s="17">
         <v>15</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="58">
         <v>640000</v>
       </c>
       <c r="D16" s="20">
@@ -1592,14 +1683,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:16366" s="16" customFormat="1">
+    <row r="17" spans="1:16366" s="16" customFormat="1" ht="15.75" thickBot="1">
       <c r="A17" s="10">
         <v>16</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="59">
         <v>20114</v>
       </c>
       <c r="D17" s="13">
@@ -1615,16 +1706,16 @@
     <row r="18" spans="1:16366" hidden="1">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="33"/>
-      <c r="F18" s="33"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="32"/>
+      <c r="F18" s="32"/>
     </row>
     <row r="19" spans="1:16366" hidden="1">
       <c r="A19" s="17"/>
       <c r="B19" s="18"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
-      <c r="F19" s="33" t="s">
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+      <c r="F19" s="32" t="s">
         <v>20</v>
       </c>
       <c r="H19" s="23" t="s">
@@ -1634,36 +1725,36 @@
     <row r="20" spans="1:16366" hidden="1">
       <c r="A20" s="17"/>
       <c r="B20" s="18"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="33"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="32"/>
       <c r="F20" s="20">
         <f>SUMPRODUCT(E2:E17,F2:F17)</f>
         <v>387020.82349999988</v>
       </c>
-      <c r="H20" s="35">
+      <c r="H20" s="34">
         <v>400330</v>
       </c>
     </row>
     <row r="21" spans="1:16366" hidden="1">
       <c r="A21" s="17"/>
       <c r="B21" s="18"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="33"/>
-      <c r="F21" s="33"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="32"/>
+      <c r="F21" s="32"/>
     </row>
     <row r="22" spans="1:16366">
       <c r="A22" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="38">
+      <c r="C22" s="31"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="37">
         <v>4</v>
       </c>
-      <c r="F22" s="39">
+      <c r="F22" s="38">
         <v>6719</v>
       </c>
       <c r="G22" s="26"/>
@@ -18029,63 +18120,63 @@
     </row>
     <row r="23" spans="1:16366">
       <c r="A23" s="17"/>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="38">
+      <c r="C23" s="31"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="37">
         <v>5</v>
       </c>
-      <c r="F23" s="39">
+      <c r="F23" s="38">
         <v>6055</v>
       </c>
     </row>
     <row r="24" spans="1:16366">
       <c r="A24" s="17"/>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="38">
+      <c r="C24" s="31"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="37">
         <v>5</v>
       </c>
-      <c r="F24" s="39">
+      <c r="F24" s="38">
         <v>6557</v>
       </c>
     </row>
     <row r="25" spans="1:16366" hidden="1">
       <c r="A25" s="17"/>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="33"/>
-      <c r="F25" s="33"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="32"/>
+      <c r="F25" s="32"/>
     </row>
     <row r="26" spans="1:16366" hidden="1">
       <c r="A26" s="17"/>
-      <c r="B26" s="41">
+      <c r="B26" s="40">
         <v>2000</v>
       </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="33"/>
-      <c r="F26" s="33"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="32"/>
+      <c r="F26" s="32"/>
     </row>
     <row r="27" spans="1:16366" hidden="1">
       <c r="A27" s="17"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="33"/>
-      <c r="F27" s="33"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="32"/>
+      <c r="F27" s="32"/>
     </row>
     <row r="28" spans="1:16366" hidden="1">
       <c r="A28" s="17"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="33"/>
-      <c r="F28" s="33" t="s">
+      <c r="B28" s="40"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="32"/>
+      <c r="F28" s="32" t="s">
         <v>20</v>
       </c>
       <c r="H28" s="23" t="s">
@@ -18094,23 +18185,23 @@
     </row>
     <row r="29" spans="1:16366" hidden="1">
       <c r="A29" s="17"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="33"/>
-      <c r="F29" s="33">
+      <c r="B29" s="40"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="32"/>
+      <c r="F29" s="32">
         <f>F20+SUMPRODUCT(E22:E24,F22:F24)</f>
         <v>476956.82349999988</v>
       </c>
-      <c r="H29" s="35">
+      <c r="H29" s="34">
         <v>400330</v>
       </c>
     </row>
     <row r="30" spans="1:16366" hidden="1">
       <c r="A30" s="17"/>
       <c r="B30" s="18"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="33"/>
-      <c r="F30" s="33"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="32"/>
+      <c r="F30" s="32"/>
     </row>
     <row r="31" spans="1:16366">
       <c r="A31" s="17" t="s">
@@ -18119,12 +18210,12 @@
       <c r="B31" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="42">
+      <c r="C31" s="31"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="41">
         <v>25</v>
       </c>
-      <c r="F31" s="39">
+      <c r="F31" s="38">
         <v>271</v>
       </c>
     </row>
@@ -18133,12 +18224,12 @@
       <c r="B32" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="43"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="45">
+      <c r="C32" s="42"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="44">
         <v>25</v>
       </c>
-      <c r="F32" s="46">
+      <c r="F32" s="45">
         <v>326</v>
       </c>
     </row>
@@ -18146,12 +18237,12 @@
       <c r="B33" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="32"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="42">
+      <c r="C33" s="31"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="41">
         <v>25</v>
       </c>
-      <c r="F33" s="39">
+      <c r="F33" s="38">
         <v>16</v>
       </c>
     </row>
@@ -18159,12 +18250,12 @@
       <c r="B34" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="32"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="42">
+      <c r="C34" s="31"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="41">
         <v>300</v>
       </c>
-      <c r="F34" s="39">
+      <c r="F34" s="38">
         <v>299</v>
       </c>
     </row>
@@ -18172,22 +18263,22 @@
       <c r="B35" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="33" t="s">
+      <c r="C35" s="31"/>
+      <c r="D35" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="33">
         <v>11454</v>
       </c>
-      <c r="F35" s="33">
+      <c r="F35" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="B36" s="18"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="33"/>
-      <c r="F36" s="33"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="32"/>
+      <c r="F36" s="32"/>
     </row>
     <row r="37" spans="1:6" s="16" customFormat="1" ht="30">
       <c r="A37" s="2" t="s">
@@ -18200,28 +18291,28 @@
       <c r="D37" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="47" t="s">
+      <c r="E37" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F37" s="48"/>
+      <c r="F37" s="47"/>
     </row>
     <row r="38" spans="1:6">
       <c r="B38" s="18"/>
-      <c r="C38" s="49">
+      <c r="C38" s="48">
         <f>F29+SUMPRODUCT(E31:E33,F31:F33)</f>
         <v>492281.82349999988</v>
       </c>
       <c r="D38" s="20">
         <v>400330</v>
       </c>
-      <c r="E38" s="50">
+      <c r="E38" s="49">
         <f>(C38-D38)/D38*100</f>
         <v>22.969006444683107</v>
       </c>
-      <c r="F38" s="51"/>
+      <c r="F38" s="50"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>